<commit_message>
Impatto errori e curva d'urgenza
</commit_message>
<xml_diff>
--- a/Project Management Sources/Curva d'urgenza.xlsx
+++ b/Project Management Sources/Curva d'urgenza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MatteoMarchesini/UUX-Project/Project Management Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FAA243-3CA6-AD48-B293-7E36F0450A7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB961736-A85C-7640-A2A3-0859845C84ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="15020" xr2:uid="{ADA57D0C-6A8F-CD4A-974D-0AC0E7DFC66E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>Utente</t>
   </si>
@@ -54,20 +54,56 @@
     <t>Daniele</t>
   </si>
   <si>
-    <t>Soddisfazione</t>
-  </si>
-  <si>
     <t>Risultati attesi</t>
   </si>
   <si>
     <t>Risultati reali</t>
+  </si>
+  <si>
+    <t>Emozione</t>
+  </si>
+  <si>
+    <t>Impatto</t>
+  </si>
+  <si>
+    <t>Implementazione</t>
+  </si>
+  <si>
+    <t>Errori</t>
+  </si>
+  <si>
+    <t>Catstrofico</t>
+  </si>
+  <si>
+    <t>Grave</t>
+  </si>
+  <si>
+    <t>Minore</t>
+  </si>
+  <si>
+    <t>Cosmetico</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>×</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -99,6 +135,20 @@
     <font>
       <sz val="18"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -268,6 +318,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -275,7 +345,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -286,6 +356,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -298,41 +371,95 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -434,7 +561,7 @@
           <c:yMode val="edge"/>
           <c:x val="6.1679247400230022E-2"/>
           <c:y val="0.10550958139368172"/>
-          <c:w val="0.78067604208224362"/>
+          <c:w val="0.67223150467704984"/>
           <c:h val="0.82851321502018438"/>
         </c:manualLayout>
       </c:layout>
@@ -445,7 +572,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Curva urgenza</c:v>
+            <c:v>Curva d'urgenza</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="38100" cap="rnd">
@@ -469,10 +596,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Foglio1!$A$1:$A$7</c:f>
+              <c:f>Foglio1!$A$1:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -480,7 +607,43 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Foglio1!$B$1:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
@@ -489,39 +652,15 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Foglio1!$B$1:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -569,7 +708,7 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1</c:v>
+                <c:v>3</c:v>
               </c:pt>
             </c:numLit>
           </c:xVal>
@@ -633,7 +772,7 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>2</c:v>
+                <c:v>1</c:v>
               </c:pt>
             </c:numLit>
           </c:yVal>
@@ -660,7 +799,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="dash"/>
+            <c:symbol val="diamond"/>
             <c:size val="12"/>
             <c:spPr>
               <a:solidFill>
@@ -679,7 +818,7 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1</c:v>
+                <c:v>4</c:v>
               </c:pt>
             </c:numLit>
           </c:xVal>
@@ -688,7 +827,7 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>2</c:v>
+                <c:v>3</c:v>
               </c:pt>
             </c:numLit>
           </c:yVal>
@@ -732,220 +871,6 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>2</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:xVal>
-          <c:yVal>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>3</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-CD4A-9E4D-BFA5-7195B4AAED40}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:v>E5</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="star"/>
-            <c:size val="12"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>1</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:xVal>
-          <c:yVal>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>1</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-CD4A-9E4D-BFA5-7195B4AAED40}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:v>E6</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="12"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>2</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:xVal>
-          <c:yVal>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>1</c:v>
-              </c:pt>
-            </c:numLit>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-CD4A-9E4D-BFA5-7195B4AAED40}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:v>E7</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="12"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:marker>
-              <c:symbol val="square"/>
-              <c:size val="12"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="60000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:ln w="41275" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000E-CD4A-9E4D-BFA5-7195B4AAED40}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:xVal>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
                 <c:v>3</c:v>
               </c:pt>
             </c:numLit>
@@ -955,14 +880,14 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>3</c:v>
+                <c:v>2</c:v>
               </c:pt>
             </c:numLit>
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-CD4A-9E4D-BFA5-7195B4AAED40}"/>
+              <c16:uniqueId val="{00000008-CD4A-9E4D-BFA5-7195B4AAED40}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -981,7 +906,8 @@
         <c:axId val="36423040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4"/>
+          <c:max val="4.5"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1114,9 +1040,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.84779822180862507"/>
+          <c:x val="0.78004951083164475"/>
           <c:y val="0.3451187985286277"/>
-          <c:w val="0.1404732569911169"/>
+          <c:w val="0.17767501133612315"/>
           <c:h val="0.45510298262042276"/>
         </c:manualLayout>
       </c:layout>
@@ -1133,7 +1059,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1149,8 +1075,8 @@
         </a:p>
       </c:txPr>
     </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:plotVisOnly val="0"/>
+    <c:dispBlanksAs val="span"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1746,16 +1672,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>104492</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>25149</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>560295</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>53163</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>314356</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>62870</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1400735</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>74706</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2080,28 +2006,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A81C49A-D5AC-CE4A-8B37-F3201402E89F}">
-  <dimension ref="A1:T31"/>
+  <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D15" zoomScale="101" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+    <sheetView tabSelected="1" topLeftCell="F32" zoomScale="68" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.83203125" customWidth="1"/>
+    <col min="24" max="24" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -2122,10 +2052,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2138,10 +2068,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>2</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2157,275 +2087,477 @@
         <v>3</v>
       </c>
       <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:20" ht="24" x14ac:dyDescent="0.3">
-      <c r="D26" s="14" t="s">
+    <row r="27" spans="4:28" ht="24" x14ac:dyDescent="0.3">
+      <c r="D27" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="21"/>
+      <c r="M27" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="16"/>
-      <c r="M26" s="14" t="s">
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="20"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="21"/>
+      <c r="W27" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="X27" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y27" s="28"/>
+      <c r="Z27" s="28"/>
+      <c r="AA27" s="28"/>
+      <c r="AB27" s="35"/>
+    </row>
+    <row r="28" spans="4:28" ht="21" x14ac:dyDescent="0.2">
+      <c r="D28" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="25"/>
+      <c r="G28" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" s="25"/>
+      <c r="I28" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="25"/>
+      <c r="K28" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="16"/>
+      <c r="M28" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="N28" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="O28" s="25"/>
+      <c r="P28" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="S28" s="25"/>
+      <c r="T28" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="W28" s="34"/>
+      <c r="X28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z28" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA28" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB28" s="9" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="27" spans="4:20" ht="21" x14ac:dyDescent="0.2">
-      <c r="D27" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="13" t="s">
+    <row r="29" spans="4:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D29" s="23"/>
+      <c r="E29" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K29" s="27"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P29" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R29" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="S29" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="T29" s="27"/>
+      <c r="W29" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="X29" s="36"/>
+      <c r="Y29" s="36"/>
+      <c r="Z29" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA29" s="36"/>
+      <c r="AB29" s="36"/>
+    </row>
+    <row r="30" spans="4:28" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D30" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1">
+        <v>3</v>
+      </c>
+      <c r="F30" s="1">
+        <v>3</v>
+      </c>
+      <c r="G30" s="1">
+        <v>3</v>
+      </c>
+      <c r="H30" s="1">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1">
+        <v>3</v>
+      </c>
+      <c r="J30" s="1">
+        <v>3</v>
+      </c>
+      <c r="K30" s="6">
+        <v>7</v>
+      </c>
+      <c r="M30" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N30" s="1">
+        <v>3</v>
+      </c>
+      <c r="O30" s="1">
+        <v>3</v>
+      </c>
+      <c r="P30" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>2</v>
+      </c>
+      <c r="R30" s="1">
+        <v>3</v>
+      </c>
+      <c r="S30" s="1">
+        <v>2</v>
+      </c>
+      <c r="T30" s="6">
+        <v>7</v>
+      </c>
+      <c r="W30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X30" s="37"/>
+      <c r="Y30" s="37"/>
+      <c r="Z30" s="37"/>
+      <c r="AA30" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB30" s="37"/>
+    </row>
+    <row r="31" spans="4:28" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="2">
+        <v>3</v>
+      </c>
+      <c r="F31" s="2">
+        <v>2</v>
+      </c>
+      <c r="G31" s="2">
+        <v>3</v>
+      </c>
+      <c r="H31" s="2">
+        <v>2</v>
+      </c>
+      <c r="I31" s="2">
+        <v>3</v>
+      </c>
+      <c r="J31" s="2">
+        <v>2</v>
+      </c>
+      <c r="K31" s="5">
+        <v>6</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="N31" s="2">
+        <v>3</v>
+      </c>
+      <c r="O31" s="2">
+        <v>2</v>
+      </c>
+      <c r="P31" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>2</v>
+      </c>
+      <c r="R31" s="2">
+        <v>3</v>
+      </c>
+      <c r="S31" s="2">
+        <v>2</v>
+      </c>
+      <c r="T31" s="5">
+        <v>6</v>
+      </c>
+      <c r="W31" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="X31" s="36"/>
+      <c r="Y31" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z31" s="36"/>
+      <c r="AA31" s="36"/>
+      <c r="AB31" s="36"/>
+    </row>
+    <row r="32" spans="4:28" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D32" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="3">
+        <v>2</v>
+      </c>
+      <c r="F32" s="3">
+        <v>2</v>
+      </c>
+      <c r="G32" s="3">
+        <v>2</v>
+      </c>
+      <c r="H32" s="3">
+        <v>2</v>
+      </c>
+      <c r="I32" s="3">
+        <v>2</v>
+      </c>
+      <c r="J32" s="3">
         <v>1</v>
       </c>
-      <c r="F27" s="9"/>
-      <c r="G27" s="13" t="s">
+      <c r="K32" s="7">
+        <v>5</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N32" s="3">
+        <v>3</v>
+      </c>
+      <c r="O32" s="3">
         <v>2</v>
       </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="J27" s="9"/>
-      <c r="K27" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="N27" s="13" t="s">
+      <c r="P32" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q32" s="3">
         <v>1</v>
       </c>
-      <c r="O27" s="9"/>
-      <c r="P27" s="13" t="s">
+      <c r="R32" s="3">
         <v>2</v>
       </c>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="S27" s="9"/>
-      <c r="T27" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="S32" s="3">
+        <v>1</v>
+      </c>
+      <c r="T32" s="7">
+        <v>5</v>
+      </c>
+      <c r="W32" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X32" s="38"/>
+      <c r="Y32" s="38"/>
+      <c r="Z32" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA32" s="38"/>
+      <c r="AB32" s="38"/>
     </row>
-    <row r="28" spans="4:20" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D28" s="11"/>
-      <c r="E28" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="K28" s="12"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="O28" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="P28" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q28" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="R28" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="S28" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="T28" s="12"/>
+    <row r="35" spans="4:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
     </row>
-    <row r="29" spans="4:20" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D29" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="1">
-        <v>3</v>
-      </c>
-      <c r="F29" s="1">
-        <v>3</v>
-      </c>
-      <c r="G29" s="1">
-        <v>3</v>
-      </c>
-      <c r="H29" s="1">
-        <v>2</v>
-      </c>
-      <c r="I29" s="1">
-        <v>3</v>
-      </c>
-      <c r="J29" s="1">
-        <v>3</v>
-      </c>
-      <c r="K29" s="5">
-        <v>7</v>
-      </c>
-      <c r="M29" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="N29" s="1">
-        <v>3</v>
-      </c>
-      <c r="O29" s="1">
-        <v>3</v>
-      </c>
-      <c r="P29" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q29" s="1">
-        <v>2</v>
-      </c>
-      <c r="R29" s="1">
-        <v>3</v>
-      </c>
-      <c r="S29" s="1">
-        <v>2</v>
-      </c>
-      <c r="T29" s="5">
-        <v>6</v>
-      </c>
+    <row r="36" spans="4:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
     </row>
-    <row r="30" spans="4:20" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D30" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="2">
-        <v>2</v>
-      </c>
-      <c r="F30" s="2">
-        <v>2</v>
-      </c>
-      <c r="G30" s="2">
-        <v>3</v>
-      </c>
-      <c r="H30" s="2">
-        <v>2</v>
-      </c>
-      <c r="I30" s="2">
-        <v>2</v>
-      </c>
-      <c r="J30" s="2">
-        <v>2</v>
-      </c>
-      <c r="K30" s="4">
-        <v>5</v>
-      </c>
-      <c r="M30" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="N30" s="2">
-        <v>2</v>
-      </c>
-      <c r="O30" s="2">
-        <v>1</v>
-      </c>
-      <c r="P30" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q30" s="2">
-        <v>2</v>
-      </c>
-      <c r="R30" s="2">
-        <v>2</v>
-      </c>
-      <c r="S30" s="2">
-        <v>1</v>
-      </c>
-      <c r="T30" s="4">
-        <v>5</v>
-      </c>
+    <row r="37" spans="4:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="D37" s="18"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="18"/>
     </row>
-    <row r="31" spans="4:20" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D31" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="3">
-        <v>1</v>
-      </c>
-      <c r="F31" s="3">
-        <v>2</v>
-      </c>
-      <c r="G31" s="3">
-        <v>2</v>
-      </c>
-      <c r="H31" s="3">
-        <v>2</v>
-      </c>
-      <c r="I31" s="3">
-        <v>2</v>
-      </c>
-      <c r="J31" s="3">
-        <v>1</v>
-      </c>
-      <c r="K31" s="6">
-        <v>3</v>
-      </c>
-      <c r="M31" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="N31" s="3">
-        <v>1</v>
-      </c>
-      <c r="O31" s="3">
-        <v>2</v>
-      </c>
-      <c r="P31" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q31" s="3">
-        <v>1</v>
-      </c>
-      <c r="R31" s="3">
-        <v>3</v>
-      </c>
-      <c r="S31" s="3">
-        <v>2</v>
-      </c>
-      <c r="T31" s="6">
-        <v>2</v>
-      </c>
+    <row r="38" spans="4:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="D38" s="14"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+    </row>
+    <row r="39" spans="4:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="D39" s="16"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="13"/>
+    </row>
+    <row r="40" spans="4:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="D40" s="14"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+    </row>
+    <row r="43" spans="4:11" ht="24" x14ac:dyDescent="0.3">
+      <c r="D43" s="29"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="21"/>
+    </row>
+    <row r="44" spans="4:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D44" s="30"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="9"/>
+    </row>
+    <row r="45" spans="4:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="D45" s="10"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="6"/>
+    </row>
+    <row r="46" spans="4:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="D46" s="11"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="5"/>
+    </row>
+    <row r="47" spans="4:11" ht="21" x14ac:dyDescent="0.2">
+      <c r="D47" s="12"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="M26:T26"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="R27:S27"/>
-    <mergeCell ref="T27:T28"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D26:K26"/>
+  <mergeCells count="22">
+    <mergeCell ref="X27:AB27"/>
+    <mergeCell ref="W27:W28"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:K43"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="M27:T27"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="T28:T29"/>
+    <mergeCell ref="D35:K35"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="K36:K37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Modello CAO=S e personas
</commit_message>
<xml_diff>
--- a/Project Management Sources/Curva d'urgenza.xlsx
+++ b/Project Management Sources/Curva d'urgenza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MatteoMarchesini/UUX-Project/Project Management Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB961736-A85C-7640-A2A3-0859845C84ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABD5689-FCBA-4249-87CD-9B631B3026B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="15020" xr2:uid="{ADA57D0C-6A8F-CD4A-974D-0AC0E7DFC66E}"/>
   </bookViews>
@@ -561,8 +561,8 @@
           <c:yMode val="edge"/>
           <c:x val="6.1679247400230022E-2"/>
           <c:y val="0.10550958139368172"/>
-          <c:w val="0.67223150467704984"/>
-          <c:h val="0.82851321502018438"/>
+          <c:w val="0.72013668574224143"/>
+          <c:h val="0.83055843424863696"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1040,9 +1040,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.78004951083164475"/>
-          <c:y val="0.3451187985286277"/>
-          <c:w val="0.17767501133612315"/>
+          <c:x val="0.81343790703243457"/>
+          <c:y val="0.34716410483113141"/>
+          <c:w val="0.17331999014692173"/>
           <c:h val="0.45510298262042276"/>
         </c:manualLayout>
       </c:layout>
@@ -1672,16 +1672,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>560295</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>249551</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>53163</xdr:rowOff>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>1400735</xdr:colOff>
+      <xdr:colOff>797128</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>74706</xdr:rowOff>
+      <xdr:rowOff>88217</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2008,8 +2008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A81C49A-D5AC-CE4A-8B37-F3201402E89F}">
   <dimension ref="A1:AB47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F32" zoomScale="68" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="J37" zoomScale="94" workbookViewId="0">
+      <selection activeCell="Y39" sqref="Y39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>